<commit_message>
Update automatico via Actualizar 06-20-2020 17-06-17
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IPSA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IPSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5D1EC234-07E2-42C1-B419-8B17816A43CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{03CA2007-DEBB-4F72-B48F-B017031F98BA}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5D1EC234-07E2-42C1-B419-8B17816A43CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{803A6CB4-C068-4921-B04B-323223CA0B4A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,7 +924,7 @@
   <dimension ref="A1:B535"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
-      <selection activeCell="B537" sqref="B537"/>
+      <selection activeCell="B538" sqref="B538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-19-2020 19-09-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IPSA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IPSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{5D1EC234-07E2-42C1-B419-8B17816A43CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5CD54669-AA5B-4D51-BAE7-5EE47B39951A}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{5D1EC234-07E2-42C1-B419-8B17816A43CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E122869-CBFC-434D-8763-73C8E90EC476}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IPSA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IPSA" localSheetId="0">IPSA!$A$1:$B$687</definedName>
+    <definedName name="IPSA" localSheetId="0">IPSA!$A$1:$B$688</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -921,13 +921,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B687"/>
+  <dimension ref="A1:B688"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B670" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B679" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B687" sqref="B687"/>
+      <selection pane="bottomRight" activeCell="B688" sqref="B688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6430,6 +6430,14 @@
         <v>4047.42</v>
       </c>
     </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="3">
+        <v>44152</v>
+      </c>
+      <c r="B688" s="4">
+        <v>4053.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-09-2021 17-06-15
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/IPSA.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/IPSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="619" documentId="8_{5D1EC234-07E2-42C1-B419-8B17816A43CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4F28D25B-CFF5-4528-AC75-52F9F1ABC63E}"/>
+  <xr:revisionPtr revIDLastSave="625" documentId="8_{5D1EC234-07E2-42C1-B419-8B17816A43CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{70864431-8555-4727-BB50-C2C4372B8187}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IPSA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="IPSA" localSheetId="0">IPSA!$A$1:$B$857</definedName>
+    <definedName name="IPSA" localSheetId="0">IPSA!$A$1:$B$858</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -941,13 +941,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B866"/>
+  <dimension ref="A1:B867"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B858" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B859" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A858" sqref="A858"/>
+      <selection pane="bottomRight" activeCell="A859" sqref="A859"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7819,8 +7819,12 @@
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A859" s="3"/>
-      <c r="B859" s="4"/>
+      <c r="A859" s="3">
+        <v>44323</v>
+      </c>
+      <c r="B859" s="4">
+        <v>4618.8</v>
+      </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A860" s="3"/>
@@ -7849,6 +7853,10 @@
     <row r="866" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A866" s="3"/>
       <c r="B866" s="4"/>
+    </row>
+    <row r="867" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A867" s="3"/>
+      <c r="B867" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>